<commit_message>
Minor changes to ease workflow.
Signed-off-by: thesteau <25945183+thesteau@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Addendum Files/mailing_list.xlsx
+++ b/Addendum Files/mailing_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steau\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steau\Documents\GitHub\Email-Sender-by-Steven-Au\Addendum Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB1F9602-14EC-4460-A7F6-50A148EE79D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A9EC8F-6495-4333-B0F3-29C6F3061462}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29535" yWindow="735" windowWidth="15300" windowHeight="8295" xr2:uid="{98C9C121-BD5D-4662-B3FD-2EE5180B95D2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>email</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>email attachment</t>
-  </si>
-  <si>
-    <t>signature</t>
   </si>
 </sst>
 </file>
@@ -400,13 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD8C39F-65C2-432D-968D-13AF0D4C2223}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,9 +421,6 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>